<commit_message>
commit 1-4-2022 Delete profile Image validate invalid email validate invalid name validate email used before
</commit_message>
<xml_diff>
--- a/src/test/testdata/Profile.xlsx
+++ b/src/test/testdata/Profile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -35,31 +35,37 @@
     <t>TestCase</t>
   </si>
   <si>
-    <t>Amiraaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01-login with new mobile number </t>
-  </si>
-  <si>
     <t>1027748599&amp;</t>
   </si>
   <si>
-    <t xml:space="preserve">02-add email used before </t>
-  </si>
-  <si>
     <t xml:space="preserve">Email </t>
   </si>
   <si>
-    <t>03-add invalid email</t>
-  </si>
-  <si>
     <t>zekrallah931@gmail.com</t>
   </si>
   <si>
     <t>kkkkkkk@kkkkkkkk</t>
   </si>
   <si>
-    <t>Amiraaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
+    <t>NewName</t>
+  </si>
+  <si>
+    <t>TestTest@gmail.com</t>
+  </si>
+  <si>
+    <t>01-Add validname and Email</t>
+  </si>
+  <si>
+    <t>Amira</t>
+  </si>
+  <si>
+    <t>02-add invalid  Name And Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03-add email used before </t>
+  </si>
+  <si>
+    <t>12&amp;</t>
   </si>
 </sst>
 </file>
@@ -107,10 +113,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -395,15 +404,15 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" customWidth="1"/>
-    <col min="2" max="2" width="49.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="33.77734375" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -418,56 +427,56 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>